<commit_message>
contraintes rampes + temps fonctionnement
</commit_message>
<xml_diff>
--- a/Donnees_Projet_Optimisation.xlsx
+++ b/Donnees_Projet_Optimisation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emac\Documents\Cours - MINES ALBI\Optimisation\Projet_final\Projet_Optimistion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emac\Desktop\ETN - OPTIMISATION\Projet_Optimistion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE0BDD5-B355-40C9-A7F4-63A365511F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A918B2F-95F1-41E1-869F-DE61898EA37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1150,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1163,69 +1163,124 @@
     <col min="5" max="7" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:18" ht="42" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:18" ht="42" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>30.4</v>
+      </c>
+      <c r="E2" s="6">
+        <v>152</v>
+      </c>
+      <c r="F2" s="6">
+        <v>40</v>
+      </c>
+      <c r="G2" s="6">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7">
+        <v>4</v>
+      </c>
+      <c r="L2" s="8">
+        <v>13.32</v>
+      </c>
+      <c r="M2" s="7">
+        <v>15</v>
+      </c>
+      <c r="N2" s="7">
+        <v>14</v>
+      </c>
+      <c r="O2" s="7">
+        <v>1430.4</v>
+      </c>
+      <c r="P2" s="7">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>1</v>
+      </c>
+      <c r="R2" s="17">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1278,105 +1333,105 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="6">
-        <v>30.4</v>
+        <v>75</v>
       </c>
       <c r="E4" s="6">
-        <v>152</v>
+        <v>350</v>
       </c>
       <c r="F4" s="6">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="G4" s="6">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H4" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I4" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J4" s="7">
         <v>8</v>
       </c>
       <c r="K4" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L4" s="8">
-        <v>13.32</v>
+        <v>20.7</v>
       </c>
       <c r="M4" s="7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N4" s="7">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="O4" s="7">
-        <v>1430.4</v>
+        <v>1725</v>
       </c>
       <c r="P4" s="7">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4" s="17">
-        <v>22</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="6">
-        <v>75</v>
+        <v>206.85</v>
       </c>
       <c r="E5" s="6">
-        <v>350</v>
+        <v>591</v>
       </c>
       <c r="F5" s="6">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="G5" s="6">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>12</v>
+      </c>
+      <c r="K5" s="7">
+        <v>10</v>
+      </c>
+      <c r="L5" s="8">
+        <v>20.93</v>
+      </c>
+      <c r="M5" s="7">
+        <v>8</v>
+      </c>
+      <c r="N5" s="7">
         <v>7</v>
       </c>
-      <c r="I5" s="6">
-        <v>7</v>
-      </c>
-      <c r="J5" s="7">
-        <v>8</v>
-      </c>
-      <c r="K5" s="7">
-        <v>8</v>
-      </c>
-      <c r="L5" s="8">
-        <v>20.7</v>
-      </c>
-      <c r="M5" s="7">
-        <v>10</v>
-      </c>
-      <c r="N5" s="7">
-        <v>9</v>
-      </c>
       <c r="O5" s="7">
-        <v>1725</v>
+        <v>3056.7</v>
       </c>
       <c r="P5" s="7">
         <v>0</v>
@@ -1385,54 +1440,54 @@
         <v>0</v>
       </c>
       <c r="R5" s="17">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="6">
-        <v>206.85</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6">
-        <v>591</v>
+        <v>60</v>
       </c>
       <c r="F6" s="6">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="G6" s="6">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="H6" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="7">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K6" s="7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L6" s="8">
-        <v>20.93</v>
+        <v>26.11</v>
       </c>
       <c r="M6" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N6" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O6" s="7">
-        <v>3056.7</v>
+        <v>437</v>
       </c>
       <c r="P6" s="7">
         <v>0</v>
@@ -1446,49 +1501,49 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
         <v>15</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>54.25</v>
+      </c>
+      <c r="E7" s="6">
+        <v>155</v>
+      </c>
+      <c r="F7" s="6">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6">
+        <v>30</v>
+      </c>
+      <c r="H7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
-        <v>12</v>
-      </c>
-      <c r="E7" s="6">
-        <v>60</v>
-      </c>
-      <c r="F7" s="6">
-        <v>60</v>
-      </c>
-      <c r="G7" s="6">
-        <v>60</v>
-      </c>
-      <c r="H7" s="6">
-        <v>1</v>
-      </c>
       <c r="I7" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" s="7">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K7" s="7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L7" s="8">
-        <v>26.11</v>
+        <v>10.52</v>
       </c>
       <c r="M7" s="7">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="N7" s="7">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="O7" s="7">
-        <v>437</v>
+        <v>312</v>
       </c>
       <c r="P7" s="7">
         <v>0</v>
@@ -1497,15 +1552,15 @@
         <v>0</v>
       </c>
       <c r="R7" s="17">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>1</v>
@@ -1547,77 +1602,77 @@
         <v>312</v>
       </c>
       <c r="P8" s="7">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="Q8" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="17">
-        <v>-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6">
-        <v>54.25</v>
+        <v>100</v>
       </c>
       <c r="E9" s="6">
-        <v>155</v>
+        <v>400</v>
       </c>
       <c r="F9" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G9" s="6">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6">
-        <v>3</v>
+        <v>6.67</v>
       </c>
       <c r="I9" s="6">
-        <v>3</v>
+        <v>6.67</v>
       </c>
       <c r="J9" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K9" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L9" s="8">
-        <v>10.52</v>
+        <v>6.02</v>
       </c>
       <c r="M9" s="7">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="N9" s="7">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7">
-        <v>312</v>
+        <v>0</v>
       </c>
       <c r="P9" s="7">
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="Q9" s="7">
         <v>1</v>
       </c>
       <c r="R9" s="17">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
@@ -1647,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="8">
-        <v>6.02</v>
+        <v>5.47</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -1665,24 +1720,24 @@
         <v>1</v>
       </c>
       <c r="R10" s="17">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="6">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E11" s="6">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -1691,19 +1746,19 @@
         <v>0</v>
       </c>
       <c r="H11" s="6">
-        <v>6.67</v>
+        <v>5</v>
       </c>
       <c r="I11" s="6">
-        <v>6.67</v>
+        <v>5</v>
       </c>
       <c r="J11" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="7">
-        <v>1</v>
-      </c>
-      <c r="L11" s="8">
-        <v>5.47</v>
+        <v>0</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0</v>
       </c>
       <c r="M11" s="7">
         <v>0</v>
@@ -1721,174 +1776,118 @@
         <v>1</v>
       </c>
       <c r="R11" s="17">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>108.5</v>
+      </c>
+      <c r="E12" s="6">
+        <v>310</v>
+      </c>
+      <c r="F12" s="6">
+        <v>60</v>
+      </c>
+      <c r="G12" s="6">
+        <v>60</v>
+      </c>
+      <c r="H12" s="6">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6">
+        <v>3</v>
+      </c>
+      <c r="J12" s="7">
+        <v>8</v>
+      </c>
+      <c r="K12" s="7">
+        <v>8</v>
+      </c>
+      <c r="L12" s="8">
+        <v>10.52</v>
+      </c>
+      <c r="M12" s="7">
+        <v>17</v>
+      </c>
+      <c r="N12" s="7">
+        <v>16</v>
+      </c>
+      <c r="O12" s="7">
+        <v>624</v>
+      </c>
+      <c r="P12" s="7">
+        <v>248</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>1</v>
+      </c>
+      <c r="R12" s="17">
         <v>10</v>
       </c>
-      <c r="B12" s="4">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="12">
+        <v>140</v>
+      </c>
+      <c r="E13" s="12">
+        <v>350</v>
+      </c>
+      <c r="F13" s="12">
+        <v>40</v>
+      </c>
+      <c r="G13" s="12">
+        <v>40</v>
+      </c>
+      <c r="H13" s="12">
         <v>4</v>
       </c>
-      <c r="D12" s="6">
-        <v>300</v>
-      </c>
-      <c r="E12" s="6">
-        <v>300</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>5</v>
-      </c>
-      <c r="I12" s="6">
-        <v>5</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0</v>
-      </c>
-      <c r="L12" s="16">
-        <v>0</v>
-      </c>
-      <c r="M12" s="7">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7">
-        <v>0</v>
-      </c>
-      <c r="P12" s="7">
-        <v>240</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>1</v>
-      </c>
-      <c r="R12" s="17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4">
-        <v>23</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6">
-        <v>108.5</v>
-      </c>
-      <c r="E13" s="6">
-        <v>310</v>
-      </c>
-      <c r="F13" s="6">
-        <v>60</v>
-      </c>
-      <c r="G13" s="6">
-        <v>60</v>
-      </c>
-      <c r="H13" s="6">
-        <v>3</v>
-      </c>
-      <c r="I13" s="6">
-        <v>3</v>
-      </c>
-      <c r="J13" s="7">
+      <c r="I13" s="12">
+        <v>4</v>
+      </c>
+      <c r="J13" s="13">
         <v>8</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="13">
         <v>8</v>
       </c>
-      <c r="L13" s="8">
-        <v>10.52</v>
-      </c>
-      <c r="M13" s="7">
-        <v>17</v>
-      </c>
-      <c r="N13" s="7">
+      <c r="L13" s="14">
+        <v>10.89</v>
+      </c>
+      <c r="M13" s="13">
         <v>16</v>
       </c>
-      <c r="O13" s="7">
-        <v>624</v>
-      </c>
-      <c r="P13" s="7">
-        <v>248</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>1</v>
-      </c>
-      <c r="R13" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="10">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10">
-        <v>23</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="12">
-        <v>140</v>
-      </c>
-      <c r="E14" s="12">
-        <v>350</v>
-      </c>
-      <c r="F14" s="12">
-        <v>40</v>
-      </c>
-      <c r="G14" s="12">
-        <v>40</v>
-      </c>
-      <c r="H14" s="12">
-        <v>4</v>
-      </c>
-      <c r="I14" s="12">
-        <v>4</v>
-      </c>
-      <c r="J14" s="13">
-        <v>8</v>
-      </c>
-      <c r="K14" s="13">
-        <v>8</v>
-      </c>
-      <c r="L14" s="14">
-        <v>10.89</v>
-      </c>
-      <c r="M14" s="13">
-        <v>16</v>
-      </c>
-      <c r="N14" s="13">
+      <c r="N13" s="13">
         <v>14</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O13" s="13">
         <v>2298</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P13" s="13">
         <v>280</v>
       </c>
-      <c r="Q14" s="13">
-        <v>1</v>
-      </c>
-      <c r="R14" s="18">
+      <c r="Q13" s="13">
+        <v>1</v>
+      </c>
+      <c r="R13" s="18">
         <v>50</v>
       </c>
     </row>

</xml_diff>